<commit_message>
add functions converting string to double, int, float, or bool
</commit_message>
<xml_diff>
--- a/test/data/ReadCellTest_Data.xlsx
+++ b/test/data/ReadCellTest_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlocal\Filter\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055EFC61-34D3-4093-BDBA-C95CFF6658C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B4DFEC-DA8F-477E-9049-BE5B7E25600A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35736" yWindow="1176" windowWidth="17280" windowHeight="9276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34452" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Hello</t>
   </si>
   <si>
     <t>adfjalfjal</t>
+  </si>
+  <si>
+    <t>234</t>
   </si>
 </sst>
 </file>
@@ -352,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -393,6 +396,11 @@
         <v>123</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>